<commit_message>
Added support for getting data from one table while column is linked
Former-commit-id: 5ec274bcc5707eae552cf325b422430338fe1c9a
</commit_message>
<xml_diff>
--- a/QSSD/testing/UniUseCase.xlsx
+++ b/QSSD/testing/UniUseCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni work\ce301_ramsay_foster_b\QSSD\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D965A212-864C-4ED9-AF7E-AD1D4B2EB80A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E50044A-3531-425B-A2D6-75B3B1B06DFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{373DEB07-F147-491C-B54D-87AD1E9DED00}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +474,14 @@
         <v>77</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>81</v>
+      </c>
+    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>0</v>

</xml_diff>